<commit_message>
adding mapping og HEBT CEBs
</commit_message>
<xml_diff>
--- a/mappingInstallationSlots.xlsx
+++ b/mappingInstallationSlots.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\emittanzeHEBT\externals\optics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\optics_updateMapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="64">
   <si>
     <t>U1_008A_QUE</t>
   </si>
@@ -156,13 +156,85 @@
   </si>
   <si>
     <t>HEBT_QUE</t>
+  </si>
+  <si>
+    <t>HEBT_CEB</t>
+  </si>
+  <si>
+    <t>H5_001B_CEB</t>
+  </si>
+  <si>
+    <t>U1_023A_CEB</t>
+  </si>
+  <si>
+    <t>H2_019A_CEB</t>
+  </si>
+  <si>
+    <t>V1_044A_CEB</t>
+  </si>
+  <si>
+    <t>T2_015A_CEB</t>
+  </si>
+  <si>
+    <t>V1_030A_CEB</t>
+  </si>
+  <si>
+    <t>HE_027A_CEB</t>
+  </si>
+  <si>
+    <t>V1_003A_CEB</t>
+  </si>
+  <si>
+    <t>T1_011A_CEB</t>
+  </si>
+  <si>
+    <t>H4_016A_CEB</t>
+  </si>
+  <si>
+    <t>Z1_011A_CEB</t>
+  </si>
+  <si>
+    <t>U1_003A_CEB</t>
+  </si>
+  <si>
+    <t>Z2_008A_CEB</t>
+  </si>
+  <si>
+    <t>H5_012A_CEB</t>
+  </si>
+  <si>
+    <r>
+      <t>T2_008</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>A_CEB</t>
+    </r>
+  </si>
+  <si>
+    <t>V2_013A_CEB</t>
+  </si>
+  <si>
+    <t>Z2_015A_CEB</t>
+  </si>
+  <si>
+    <t>U1_011A_CEB</t>
+  </si>
+  <si>
+    <t>U2_013A_CEB</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,6 +244,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -199,9 +278,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -482,58 +562,74 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B43"/>
+  <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -541,135 +637,183 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -677,7 +821,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -685,7 +829,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -693,7 +837,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -701,7 +845,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -709,7 +853,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -717,7 +861,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -725,7 +869,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -733,7 +877,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -741,7 +885,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
updating mapping of instalattion slots with SYNCHRO elements
</commit_message>
<xml_diff>
--- a/mappingInstallationSlots.xlsx
+++ b/mappingInstallationSlots.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="131">
   <si>
     <t>U1_008A_QUE</t>
   </si>
@@ -229,12 +229,213 @@
   <si>
     <t>U2_013A_CEB</t>
   </si>
+  <si>
+    <t>SYNCH_MBS</t>
+  </si>
+  <si>
+    <t>SYNCH_QUS</t>
+  </si>
+  <si>
+    <t>SYNCH_CSH</t>
+  </si>
+  <si>
+    <t>SYNCH_CSV</t>
+  </si>
+  <si>
+    <t>SYNCH_SX</t>
+  </si>
+  <si>
+    <t>S0_001A_MBS</t>
+  </si>
+  <si>
+    <t>S1_001A_MBS</t>
+  </si>
+  <si>
+    <t>S2_001A_MBS</t>
+  </si>
+  <si>
+    <t>S3_001A_MBS</t>
+  </si>
+  <si>
+    <t>S4_001A_MBS</t>
+  </si>
+  <si>
+    <t>S5_001A_MBS</t>
+  </si>
+  <si>
+    <t>S6_001A_MBS</t>
+  </si>
+  <si>
+    <t>S7_001A_MBS</t>
+  </si>
+  <si>
+    <t>S8_001A_MBS</t>
+  </si>
+  <si>
+    <t>S9_001A_MBS</t>
+  </si>
+  <si>
+    <t>SA_001A_MBS</t>
+  </si>
+  <si>
+    <t>SB_001A_MBS</t>
+  </si>
+  <si>
+    <t>SC_001A_MBS</t>
+  </si>
+  <si>
+    <t>SD_001A_MBS</t>
+  </si>
+  <si>
+    <t>SE_001A_MBS</t>
+  </si>
+  <si>
+    <t>SF_001A_MBS</t>
+  </si>
+  <si>
+    <t>S0_005A_QUS</t>
+  </si>
+  <si>
+    <t>S0_031A_QUS</t>
+  </si>
+  <si>
+    <t>S1_007A_QUS</t>
+  </si>
+  <si>
+    <t>S2_005A_QUS</t>
+  </si>
+  <si>
+    <t>S2_021A_QUS</t>
+  </si>
+  <si>
+    <t>S3_016A_QUS</t>
+  </si>
+  <si>
+    <t>S4_005A_QUS</t>
+  </si>
+  <si>
+    <t>S4_024A_QUS</t>
+  </si>
+  <si>
+    <t>S5_007A_QUS</t>
+  </si>
+  <si>
+    <t>S6_005A_QUS</t>
+  </si>
+  <si>
+    <t>S6_019A_QUS</t>
+  </si>
+  <si>
+    <t>S7_007A_QUS</t>
+  </si>
+  <si>
+    <t>S8_005A_QUS</t>
+  </si>
+  <si>
+    <t>S8_037A_QUS</t>
+  </si>
+  <si>
+    <t>S9_007A_QUS</t>
+  </si>
+  <si>
+    <t>SA_005A_QUS</t>
+  </si>
+  <si>
+    <t>SA_020A_QUS</t>
+  </si>
+  <si>
+    <t>SB_012A_QUS</t>
+  </si>
+  <si>
+    <t>SC_005A_QUS</t>
+  </si>
+  <si>
+    <t>SC_025A_QUS</t>
+  </si>
+  <si>
+    <t>SD_007A_QUS</t>
+  </si>
+  <si>
+    <t>SE_005A_QUS</t>
+  </si>
+  <si>
+    <t>SE_018A_QUS</t>
+  </si>
+  <si>
+    <t>SF_007A_QUS</t>
+  </si>
+  <si>
+    <t>S0_029A_CSH</t>
+  </si>
+  <si>
+    <t>S2_008A_CSH</t>
+  </si>
+  <si>
+    <t>S4_008A_CSH</t>
+  </si>
+  <si>
+    <t>S6_014A_CSH</t>
+  </si>
+  <si>
+    <t>S8_008A_CSH</t>
+  </si>
+  <si>
+    <t>S8_035A_CSH</t>
+  </si>
+  <si>
+    <t>SA_008A_CSH</t>
+  </si>
+  <si>
+    <t>SC_008A_CSH</t>
+  </si>
+  <si>
+    <t>SC_021A_CSH</t>
+  </si>
+  <si>
+    <t>S1_005A_CSV</t>
+  </si>
+  <si>
+    <t>S3_005A_CSV</t>
+  </si>
+  <si>
+    <t>S5_005A_CSV</t>
+  </si>
+  <si>
+    <t>S7_005A_CSV</t>
+  </si>
+  <si>
+    <t>S9_005A_CSV</t>
+  </si>
+  <si>
+    <t>SB_007A_CSV</t>
+  </si>
+  <si>
+    <t>SD_005A_CSV</t>
+  </si>
+  <si>
+    <t>SF_005A_CSV</t>
+  </si>
+  <si>
+    <t>S2_019A_SXC</t>
+  </si>
+  <si>
+    <t>S5_012A_SXC</t>
+  </si>
+  <si>
+    <t>S8_028A_SXR</t>
+  </si>
+  <si>
+    <t>SA_018A_SXC</t>
+  </si>
+  <si>
+    <t>SD_014A_SXC</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -244,13 +445,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -562,19 +756,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>42</v>
       </c>
@@ -584,8 +783,23 @@
       <c r="C1" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -595,8 +809,11 @@
       <c r="C2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -606,8 +823,17 @@
       <c r="C3" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>115</v>
+      </c>
+      <c r="G3" t="s">
+        <v>125</v>
+      </c>
+      <c r="H3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -617,8 +843,17 @@
       <c r="C4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>97</v>
+      </c>
+      <c r="G4" t="s">
+        <v>123</v>
+      </c>
+      <c r="H4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -628,16 +863,43 @@
       <c r="C5" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E5" t="s">
+        <v>90</v>
+      </c>
+      <c r="F5" t="s">
+        <v>110</v>
+      </c>
+      <c r="G5" t="s">
+        <v>120</v>
+      </c>
+      <c r="H5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E6" t="s">
+        <v>87</v>
+      </c>
+      <c r="F6" t="s">
+        <v>111</v>
+      </c>
+      <c r="G6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -647,8 +909,23 @@
       <c r="C7" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E7" t="s">
+        <v>102</v>
+      </c>
+      <c r="F7" t="s">
+        <v>116</v>
+      </c>
+      <c r="G7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -658,8 +935,20 @@
       <c r="C8" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>78</v>
+      </c>
+      <c r="E8" t="s">
+        <v>94</v>
+      </c>
+      <c r="F8" t="s">
+        <v>117</v>
+      </c>
+      <c r="G8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -669,8 +958,17 @@
       <c r="C9" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>95</v>
+      </c>
+      <c r="F9" t="s">
+        <v>114</v>
+      </c>
+      <c r="G9" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -680,8 +978,20 @@
       <c r="C10" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>75</v>
+      </c>
+      <c r="E10" t="s">
+        <v>91</v>
+      </c>
+      <c r="F10" t="s">
+        <v>109</v>
+      </c>
+      <c r="G10" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -691,8 +1001,17 @@
       <c r="C11" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>80</v>
+      </c>
+      <c r="E11" t="s">
+        <v>86</v>
+      </c>
+      <c r="F11" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -702,8 +1021,17 @@
       <c r="C12" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E12" t="s">
+        <v>96</v>
+      </c>
+      <c r="F12" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -713,8 +1041,14 @@
       <c r="C13" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>79</v>
+      </c>
+      <c r="E13" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -724,8 +1058,14 @@
       <c r="C14" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>82</v>
+      </c>
+      <c r="E14" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -735,8 +1075,14 @@
       <c r="C15" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>73</v>
+      </c>
+      <c r="E15" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -746,8 +1092,11 @@
       <c r="C16" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -757,8 +1106,14 @@
       <c r="C17" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>77</v>
+      </c>
+      <c r="E17" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -768,8 +1123,14 @@
       <c r="C18" s="2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>72</v>
+      </c>
+      <c r="E18" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -779,8 +1140,14 @@
       <c r="C19" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>71</v>
+      </c>
+      <c r="E19" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -790,8 +1157,14 @@
       <c r="C20" s="2" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>83</v>
+      </c>
+      <c r="E20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -801,8 +1174,11 @@
       <c r="C21" s="2" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -812,48 +1188,72 @@
       <c r="C22" s="2" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>84</v>
+      </c>
+      <c r="E23" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>81</v>
+      </c>
+      <c r="E24" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -861,7 +1261,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -869,7 +1269,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -877,7 +1277,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -885,7 +1285,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>

</xml_diff>